<commit_message>
Perubahan 17 Oktober 2022
</commit_message>
<xml_diff>
--- a/Source/Data/Jumlah Desa_Kelurahan Menurut Provinsi.xlsx
+++ b/Source/Data/Jumlah Desa_Kelurahan Menurut Provinsi.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lydia.natalia\Desktop\INSTALASI DA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lydia.natalia\Desktop\INSTALASI DA\Git Project\Source\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A80322-2E57-4B0B-B0F6-A456F488B477}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2AA41F-14D0-40DE-A383-D568DEF8CA38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Worksheet" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="100">
   <si>
     <t>Aceh</t>
   </si>
@@ -215,13 +216,118 @@
   </si>
   <si>
     <t>6513</t>
+  </si>
+  <si>
+    <t>ACEH</t>
+  </si>
+  <si>
+    <t>SUMATERA UTARA</t>
+  </si>
+  <si>
+    <t>SUMATERA BARAT</t>
+  </si>
+  <si>
+    <t>RIAU</t>
+  </si>
+  <si>
+    <t>JAMBI</t>
+  </si>
+  <si>
+    <t>SUMATERA SELATAN</t>
+  </si>
+  <si>
+    <t>BENGKULU</t>
+  </si>
+  <si>
+    <t>LAMPUNG</t>
+  </si>
+  <si>
+    <t>KEP. BANGKA BELITUNG</t>
+  </si>
+  <si>
+    <t>KEP. RIAU</t>
+  </si>
+  <si>
+    <t>DKI JAKARTA</t>
+  </si>
+  <si>
+    <t>JAWA BARAT</t>
+  </si>
+  <si>
+    <t>JAWA TENGAH</t>
+  </si>
+  <si>
+    <t>DI YOGYAKARTA</t>
+  </si>
+  <si>
+    <t>JAWA TIMUR</t>
+  </si>
+  <si>
+    <t>BANTEN</t>
+  </si>
+  <si>
+    <t>BALI</t>
+  </si>
+  <si>
+    <t>NUSA TENGGARA BARAT</t>
+  </si>
+  <si>
+    <t>NUSA TENGGARA TIMUR</t>
+  </si>
+  <si>
+    <t>KALIMANTAN BARAT</t>
+  </si>
+  <si>
+    <t>KALIMANTAN TENGAH</t>
+  </si>
+  <si>
+    <t>KALIMANTAN SELATAN</t>
+  </si>
+  <si>
+    <t>KALIMANTAN TIMUR</t>
+  </si>
+  <si>
+    <t>KALIMANTAN UTARA</t>
+  </si>
+  <si>
+    <t>SULAWESI UTARA</t>
+  </si>
+  <si>
+    <t>SULAWESI TENGAH</t>
+  </si>
+  <si>
+    <t>SULAWESI SELATAN</t>
+  </si>
+  <si>
+    <t>SULAWESI TENGGARA</t>
+  </si>
+  <si>
+    <t>GORONTALO</t>
+  </si>
+  <si>
+    <t>SULAWESI BARAT</t>
+  </si>
+  <si>
+    <t>MALUKU</t>
+  </si>
+  <si>
+    <t>MALUKU UTARA</t>
+  </si>
+  <si>
+    <t>PAPUA BARAT</t>
+  </si>
+  <si>
+    <t>PAPUA</t>
+  </si>
+  <si>
+    <t>INDONESIA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -239,6 +345,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -258,8 +371,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -272,8 +386,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{536C8B20-00D3-4C9A-90E1-45AFDB02D07A}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
@@ -574,11 +689,750 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03D40968-F327-4738-BEC6-9E6E99CCC3E7}">
+  <dimension ref="A1:F36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="4">
+        <v>2014</v>
+      </c>
+      <c r="C1" s="4">
+        <v>2018</v>
+      </c>
+      <c r="D1" s="4">
+        <v>2019</v>
+      </c>
+      <c r="E1" s="4">
+        <v>2020</v>
+      </c>
+      <c r="F1" s="4">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="3">
+        <v>6513</v>
+      </c>
+      <c r="C2" s="3">
+        <v>6514</v>
+      </c>
+      <c r="D2" s="3">
+        <v>6516</v>
+      </c>
+      <c r="E2" s="3">
+        <v>6516</v>
+      </c>
+      <c r="F2" s="3">
+        <v>6516</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="3">
+        <v>6015</v>
+      </c>
+      <c r="C3" s="3">
+        <v>6136</v>
+      </c>
+      <c r="D3" s="3">
+        <v>6132</v>
+      </c>
+      <c r="E3" s="3">
+        <v>6132</v>
+      </c>
+      <c r="F3" s="3">
+        <v>6132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1145</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1159</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1159</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1159</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1835</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1875</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1875</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1873</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1876</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1551</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1562</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1562</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1562</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1562</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="3">
+        <v>3257</v>
+      </c>
+      <c r="C7" s="3">
+        <v>3266</v>
+      </c>
+      <c r="D7" s="3">
+        <v>3289</v>
+      </c>
+      <c r="E7" s="3">
+        <v>3289</v>
+      </c>
+      <c r="F7" s="3">
+        <v>3289</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1524</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1514</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1514</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1514</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1514</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="3">
+        <v>2631</v>
+      </c>
+      <c r="C9" s="3">
+        <v>2653</v>
+      </c>
+      <c r="D9" s="3">
+        <v>2654</v>
+      </c>
+      <c r="E9" s="3">
+        <v>2654</v>
+      </c>
+      <c r="F9" s="3">
+        <v>2654</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="3">
+        <v>381</v>
+      </c>
+      <c r="C10" s="3">
+        <v>391</v>
+      </c>
+      <c r="D10" s="3">
+        <v>391</v>
+      </c>
+      <c r="E10" s="3">
+        <v>393</v>
+      </c>
+      <c r="F10" s="3">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="3">
+        <v>416</v>
+      </c>
+      <c r="C11" s="3">
+        <v>416</v>
+      </c>
+      <c r="D11" s="3">
+        <v>417</v>
+      </c>
+      <c r="E11" s="3">
+        <v>417</v>
+      </c>
+      <c r="F11" s="3">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" s="3">
+        <v>267</v>
+      </c>
+      <c r="C12" s="3">
+        <v>267</v>
+      </c>
+      <c r="D12" s="3">
+        <v>267</v>
+      </c>
+      <c r="E12" s="3">
+        <v>267</v>
+      </c>
+      <c r="F12" s="3">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" s="3">
+        <v>5962</v>
+      </c>
+      <c r="C13" s="3">
+        <v>5957</v>
+      </c>
+      <c r="D13" s="3">
+        <v>5957</v>
+      </c>
+      <c r="E13" s="3">
+        <v>5957</v>
+      </c>
+      <c r="F13" s="3">
+        <v>5957</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="3">
+        <v>8578</v>
+      </c>
+      <c r="C14" s="3">
+        <v>8559</v>
+      </c>
+      <c r="D14" s="3">
+        <v>8562</v>
+      </c>
+      <c r="E14" s="3">
+        <v>8562</v>
+      </c>
+      <c r="F14" s="3">
+        <v>8562</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" s="3">
+        <v>438</v>
+      </c>
+      <c r="C15" s="3">
+        <v>438</v>
+      </c>
+      <c r="D15" s="3">
+        <v>438</v>
+      </c>
+      <c r="E15" s="3">
+        <v>438</v>
+      </c>
+      <c r="F15" s="3">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16" s="3">
+        <v>8499</v>
+      </c>
+      <c r="C16" s="3">
+        <v>8501</v>
+      </c>
+      <c r="D16" s="3">
+        <v>8496</v>
+      </c>
+      <c r="E16" s="3">
+        <v>8496</v>
+      </c>
+      <c r="F16" s="3">
+        <v>8496</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1551</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1552</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1552</v>
+      </c>
+      <c r="E17" s="3">
+        <v>1552</v>
+      </c>
+      <c r="F17" s="3">
+        <v>1552</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" s="3">
+        <v>716</v>
+      </c>
+      <c r="C18" s="3">
+        <v>716</v>
+      </c>
+      <c r="D18" s="3">
+        <v>716</v>
+      </c>
+      <c r="E18" s="3">
+        <v>716</v>
+      </c>
+      <c r="F18" s="3">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" s="3">
+        <v>1141</v>
+      </c>
+      <c r="C19" s="3">
+        <v>1143</v>
+      </c>
+      <c r="D19" s="3">
+        <v>1143</v>
+      </c>
+      <c r="E19" s="3">
+        <v>1143</v>
+      </c>
+      <c r="F19" s="3">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>83</v>
+      </c>
+      <c r="B20" s="3">
+        <v>3270</v>
+      </c>
+      <c r="C20" s="3">
+        <v>3353</v>
+      </c>
+      <c r="D20" s="3">
+        <v>3353</v>
+      </c>
+      <c r="E20" s="3">
+        <v>3353</v>
+      </c>
+      <c r="F20" s="3">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" s="3">
+        <v>2005</v>
+      </c>
+      <c r="C21" s="3">
+        <v>2132</v>
+      </c>
+      <c r="D21" s="3">
+        <v>2132</v>
+      </c>
+      <c r="E21" s="3">
+        <v>2137</v>
+      </c>
+      <c r="F21" s="3">
+        <v>2137</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" s="3">
+        <v>1569</v>
+      </c>
+      <c r="C22" s="3">
+        <v>1576</v>
+      </c>
+      <c r="D22" s="3">
+        <v>1576</v>
+      </c>
+      <c r="E22" s="3">
+        <v>1576</v>
+      </c>
+      <c r="F22" s="3">
+        <v>1576</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>86</v>
+      </c>
+      <c r="B23" s="3">
+        <v>2009</v>
+      </c>
+      <c r="C23" s="3">
+        <v>2008</v>
+      </c>
+      <c r="D23" s="3">
+        <v>2008</v>
+      </c>
+      <c r="E23" s="3">
+        <v>2007</v>
+      </c>
+      <c r="F23" s="3">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>87</v>
+      </c>
+      <c r="B24" s="3">
+        <v>1026</v>
+      </c>
+      <c r="C24" s="3">
+        <v>1038</v>
+      </c>
+      <c r="D24" s="3">
+        <v>1038</v>
+      </c>
+      <c r="E24" s="3">
+        <v>1038</v>
+      </c>
+      <c r="F24" s="3">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>88</v>
+      </c>
+      <c r="B25" s="3">
+        <v>479</v>
+      </c>
+      <c r="C25" s="3">
+        <v>482</v>
+      </c>
+      <c r="D25" s="3">
+        <v>482</v>
+      </c>
+      <c r="E25" s="3">
+        <v>482</v>
+      </c>
+      <c r="F25" s="3">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>89</v>
+      </c>
+      <c r="B26" s="3">
+        <v>1830</v>
+      </c>
+      <c r="C26" s="3">
+        <v>1838</v>
+      </c>
+      <c r="D26" s="3">
+        <v>1839</v>
+      </c>
+      <c r="E26" s="3">
+        <v>1840</v>
+      </c>
+      <c r="F26" s="3">
+        <v>1840</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>90</v>
+      </c>
+      <c r="B27" s="3">
+        <v>1985</v>
+      </c>
+      <c r="C27" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D27" s="3">
+        <v>2020</v>
+      </c>
+      <c r="E27" s="3">
+        <v>2020</v>
+      </c>
+      <c r="F27" s="3">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28" s="3">
+        <v>3030</v>
+      </c>
+      <c r="C28" s="3">
+        <v>3049</v>
+      </c>
+      <c r="D28" s="3">
+        <v>3051</v>
+      </c>
+      <c r="E28" s="3">
+        <v>3051</v>
+      </c>
+      <c r="F28" s="3">
+        <v>3051</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>92</v>
+      </c>
+      <c r="B29" s="3">
+        <v>2268</v>
+      </c>
+      <c r="C29" s="3">
+        <v>2356</v>
+      </c>
+      <c r="D29" s="3">
+        <v>2317</v>
+      </c>
+      <c r="E29" s="3">
+        <v>2316</v>
+      </c>
+      <c r="F29" s="3">
+        <v>2309</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30" s="3">
+        <v>735</v>
+      </c>
+      <c r="C30" s="3">
+        <v>734</v>
+      </c>
+      <c r="D30" s="3">
+        <v>734</v>
+      </c>
+      <c r="E30" s="3">
+        <v>734</v>
+      </c>
+      <c r="F30" s="3">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>94</v>
+      </c>
+      <c r="B31" s="3">
+        <v>649</v>
+      </c>
+      <c r="C31" s="3">
+        <v>650</v>
+      </c>
+      <c r="D31" s="3">
+        <v>650</v>
+      </c>
+      <c r="E31" s="3">
+        <v>650</v>
+      </c>
+      <c r="F31" s="3">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>95</v>
+      </c>
+      <c r="B32" s="3">
+        <v>1190</v>
+      </c>
+      <c r="C32" s="3">
+        <v>1240</v>
+      </c>
+      <c r="D32" s="3">
+        <v>1240</v>
+      </c>
+      <c r="E32" s="3">
+        <v>1248</v>
+      </c>
+      <c r="F32" s="3">
+        <v>1248</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>96</v>
+      </c>
+      <c r="B33" s="3">
+        <v>1196</v>
+      </c>
+      <c r="C33" s="3">
+        <v>1195</v>
+      </c>
+      <c r="D33" s="3">
+        <v>1199</v>
+      </c>
+      <c r="E33" s="3">
+        <v>1199</v>
+      </c>
+      <c r="F33" s="3">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>97</v>
+      </c>
+      <c r="B34" s="3">
+        <v>1590</v>
+      </c>
+      <c r="C34" s="3">
+        <v>1878</v>
+      </c>
+      <c r="D34" s="3">
+        <v>1986</v>
+      </c>
+      <c r="E34" s="3">
+        <v>1986</v>
+      </c>
+      <c r="F34" s="3">
+        <v>1987</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>98</v>
+      </c>
+      <c r="B35" s="3">
+        <v>4375</v>
+      </c>
+      <c r="C35" s="3">
+        <v>5538</v>
+      </c>
+      <c r="D35" s="3">
+        <v>5555</v>
+      </c>
+      <c r="E35" s="3">
+        <v>5554</v>
+      </c>
+      <c r="F35" s="3">
+        <v>5560</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>99</v>
+      </c>
+      <c r="B36" s="3">
+        <v>81626</v>
+      </c>
+      <c r="C36" s="3">
+        <v>83706</v>
+      </c>
+      <c r="D36" s="3">
+        <v>83820</v>
+      </c>
+      <c r="E36" s="3">
+        <v>83831</v>
+      </c>
+      <c r="F36" s="3">
+        <v>83843</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H36" sqref="A1:H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>